<commit_message>
minor changes to test classes
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -427,9 +427,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -473,17 +473,64 @@
           <t>AAPL</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>IBKR</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>20</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>2611</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>130.55</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
+        <v>190.6900024414062</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3813.800048828125</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1202.800048828125</v>
+      </c>
+      <c r="I2" t="n">
         <v>8367</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>GME</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>IBKR</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1002</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>22.96999931335449</v>
+      </c>
+      <c r="G3" t="n">
+        <v>229.6999931335449</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-772.3000068664551</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -515,10 +562,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -679,6 +726,44 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>45124</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>GameStop</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>GME</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F5" t="n">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <f>F5*E5</f>
+        <v/>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Speculative</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added currency and is_open property
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -478,26 +478,34 @@
           <t>IBKR</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>20</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>2611</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>130.55</v>
       </c>
-      <c r="F2" t="n">
-        <v>190.6900024414062</v>
-      </c>
       <c r="G2" t="n">
-        <v>3813.800048828125</v>
+        <v>193.9900054931641</v>
       </c>
       <c r="H2" t="n">
-        <v>1202.800048828125</v>
+        <v>3879.800109863281</v>
       </c>
       <c r="I2" t="n">
+        <v>1268.800109863281</v>
+      </c>
+      <c r="J2" t="n">
         <v>8367</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -511,26 +519,34 @@
           <t>IBKR</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>10</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>1002</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" t="n">
-        <v>22.96999931335449</v>
-      </c>
       <c r="G3" t="n">
-        <v>229.6999931335449</v>
+        <v>22.81999969482422</v>
       </c>
       <c r="H3" t="n">
-        <v>-772.3000068664551</v>
+        <v>228.1999969482422</v>
       </c>
       <c r="I3" t="n">
+        <v>-773.8000030517578</v>
+      </c>
+      <c r="J3" t="n">
         <v>0</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated logic to force updating positions header
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -430,40 +430,65 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
-  <cols>
-    <col width="29.33203125" customWidth="1" min="2" max="2"/>
-    <col width="26.33203125" customWidth="1" min="3" max="3"/>
-    <col width="22.33203125" customWidth="1" min="4" max="4"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ticker</t>
+          <t>Ticker</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>pos_amount</t>
+          <t>Broker</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>total_cost</t>
+          <t>Currency</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>average_cost</t>
+          <t>Amount</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>realized_pnl</t>
+          <t>Cost Basis</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Unit Cost Basis</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Last Price</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Market Value</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Unreal. PnL</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Real. PnL</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Active</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
logic to take portfolio snapshots
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -493,13 +493,13 @@
         <v>130.55</v>
       </c>
       <c r="G2" t="n">
-        <v>193.9900054931641</v>
+        <v>195.6349945068359</v>
       </c>
       <c r="H2" t="n">
-        <v>3879.800109863281</v>
+        <v>3912.699890136719</v>
       </c>
       <c r="I2" t="n">
-        <v>1268.800109863281</v>
+        <v>1301.699890136719</v>
       </c>
       <c r="J2" t="n">
         <v>8367</v>
@@ -534,13 +534,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>22.81999969482422</v>
+        <v>23.28000068664551</v>
       </c>
       <c r="H3" t="n">
-        <v>228.1999969482422</v>
+        <v>232.8000068664551</v>
       </c>
       <c r="I3" t="n">
-        <v>-773.8000030517578</v>
+        <v>-769.1999931335449</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
changes for testing purposes
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\coding\portfolio_tracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utezstage198\Documents\strategies_py\portfolio_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414C2DD3-439C-4970-8411-9BBE7C8159A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A691275-5482-4930-B93A-43FBBFAD0CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-450" yWindow="1560" windowWidth="28800" windowHeight="12975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Positions" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
   <si>
     <t>Ticker</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Market Value</t>
   </si>
   <si>
-    <t>Unreal. PnL</t>
-  </si>
-  <si>
     <t>Real. PnL</t>
   </si>
   <si>
@@ -94,27 +91,18 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
     <t>Price</t>
   </si>
   <si>
-    <t>Notional</t>
-  </si>
-  <si>
     <t>Transaction Costs</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Apple</t>
-  </si>
-  <si>
     <t>Buy</t>
   </si>
   <si>
@@ -124,13 +112,7 @@
     <t>Sell</t>
   </si>
   <si>
-    <t>GameStop</t>
-  </si>
-  <si>
     <t>Speculative</t>
-  </si>
-  <si>
-    <t>Disney</t>
   </si>
   <si>
     <t xml:space="preserve">Unit Cost Basis </t>
@@ -486,76 +468,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="B4" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
       <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -563,45 +537,37 @@
       <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>2611</v>
+      </c>
+      <c r="F2">
+        <v>130.55000000000001</v>
+      </c>
+      <c r="G2">
+        <v>180.05499267578119</v>
+      </c>
+      <c r="H2">
+        <v>3601.099853515625</v>
+      </c>
+      <c r="I2">
+        <v>12250</v>
+      </c>
+      <c r="J2">
+        <v>13240.099853515625</v>
+      </c>
+      <c r="K2">
+        <v>73.533644675749784</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>15</v>
-      </c>
-      <c r="E2">
-        <v>20</v>
-      </c>
-      <c r="F2">
-        <v>2611</v>
-      </c>
-      <c r="G2">
-        <v>130.55000000000001</v>
-      </c>
-      <c r="H2">
-        <v>180.05499267578119</v>
-      </c>
-      <c r="I2">
-        <v>3601.099853515625</v>
-      </c>
-      <c r="J2">
-        <v>990.099853515625</v>
-      </c>
-      <c r="K2">
-        <v>12250</v>
-      </c>
-      <c r="L2">
-        <f>J2+K2</f>
-        <v>13240.099853515625</v>
-      </c>
-      <c r="M2">
-        <f>L2/H2</f>
-        <v>73.533644675749784</v>
-      </c>
-      <c r="N2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -609,45 +575,37 @@
       <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
+      <c r="D3">
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>1002</v>
       </c>
       <c r="F3">
-        <v>1002</v>
+        <v>100.2</v>
       </c>
       <c r="G3">
-        <v>100.2</v>
+        <v>17.139999389648441</v>
       </c>
       <c r="H3">
-        <v>17.139999389648441</v>
+        <v>171.3999938964844</v>
       </c>
       <c r="I3">
-        <v>171.3999938964844</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>-830.60000610351563</v>
       </c>
       <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L6" si="0">J3+K3</f>
-        <v>-830.60000610351563</v>
-      </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M6" si="1">L3/H3</f>
         <v>-48.459745372286861</v>
       </c>
-      <c r="N3" t="b">
+      <c r="L3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -655,59 +613,47 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
+      <c r="D4">
+        <v>290</v>
       </c>
       <c r="E4">
-        <v>290</v>
+        <v>25108.4175</v>
       </c>
       <c r="F4">
-        <v>25108.4175</v>
+        <v>86.580749999999995</v>
       </c>
       <c r="G4">
-        <v>86.580749999999995</v>
+        <v>86.205001831054688</v>
       </c>
       <c r="H4">
-        <v>86.205001831054688</v>
+        <v>24999.450531005859</v>
       </c>
       <c r="I4">
-        <v>24999.450531005859</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>-108.9669689941402</v>
       </c>
       <c r="K4">
+        <v>-1.2640446224651165</v>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J5">
         <v>0</v>
       </c>
-      <c r="L4">
-        <f t="shared" si="0"/>
-        <v>-108.9669689941402</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="1"/>
-        <v>-1.2640446224651165</v>
-      </c>
-      <c r="N4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L5">
-        <f t="shared" si="0"/>
+      <c r="K5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J6">
         <v>0</v>
       </c>
-      <c r="M5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M6" t="e">
-        <f t="shared" si="1"/>
+      <c r="K6" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -732,80 +678,72 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="B4" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45119</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -814,45 +752,36 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
+      <c r="G2">
+        <v>30</v>
       </c>
       <c r="H2">
-        <v>30</v>
+        <v>150.5</v>
       </c>
       <c r="I2">
-        <v>150.5</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <f>I2*H2</f>
-        <v>4515</v>
+        <v>4516</v>
       </c>
       <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <f>J2+K2</f>
-        <v>4516</v>
-      </c>
-      <c r="M2">
-        <f>L2/H2</f>
         <v>150.53333333333333</v>
       </c>
-      <c r="N2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45122</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -861,42 +790,33 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
+      <c r="G3">
+        <v>50</v>
       </c>
       <c r="H3">
-        <v>50</v>
+        <v>130.5</v>
       </c>
       <c r="I3">
-        <v>130.5</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <f>I3*H3</f>
-        <v>6525</v>
+        <v>6526</v>
       </c>
       <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L6" si="0">J3+K3</f>
-        <v>6526</v>
-      </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M6" si="1">L3/H3</f>
         <v>130.52000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45124</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -905,127 +825,100 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
+      <c r="G4">
+        <v>60</v>
       </c>
       <c r="H4">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="I4">
-        <v>140</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <f>I4*H4</f>
-        <v>8400</v>
+        <v>8401</v>
       </c>
       <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="0"/>
-        <v>8401</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="1"/>
         <v>140.01666666666668</v>
       </c>
-      <c r="N4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45124</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
+      <c r="G5">
+        <v>10</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="I5">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <f>I5*H5</f>
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="0"/>
-        <v>1002</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="1"/>
         <v>100.2</v>
       </c>
-      <c r="N5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45161</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
+      <c r="G6">
+        <v>290</v>
       </c>
       <c r="H6">
-        <v>290</v>
+        <v>86.15</v>
       </c>
       <c r="I6">
-        <v>86.15</v>
+        <v>124.9175</v>
       </c>
       <c r="J6">
-        <f>I6*H6</f>
-        <v>24983.5</v>
+        <v>25108.4175</v>
       </c>
       <c r="K6">
-        <v>124.9175</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>25108.4175</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="1"/>
         <v>86.580749999999995</v>
       </c>
     </row>

</xml_diff>